<commit_message>
new change to correct prices of barcodes
</commit_message>
<xml_diff>
--- a/App/django_files/ans correctBarcodes.xlsx
+++ b/App/django_files/ans correctBarcodes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,6 +540,2076 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>85602</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری هیرو 12 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>84477</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری سوئیت لاو 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>84476</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری فارنهایت 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>84475</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری اسپیس 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>84474</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری گودگرل 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>84473</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری الین 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>84472</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری دیزایر بلو 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>84471</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری جادور 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>84470</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری اکلت 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>84454</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری هوگو بوس 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>84453</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری ورساچ پورهوم 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>84452</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری مفیستو کازاموراتی 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>84451</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری لیتون مارلی 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>84450</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری لولیتا 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>84449</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری لالیک نویر 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>84448</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری رجینا 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>84447</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری رالف صورتی 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>84446</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری ترنزی 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>84445</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری اسپلندور مشکی 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>84444</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری اچ ام وی ای پی 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>82705</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری ناشا 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>82704</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری تارا 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>82703</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری آیسو 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>82702</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری آتس سا 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>82701</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری آتس سا 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>82700</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری آتس سا 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>82699</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری آیهان 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>82698</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری بست اف کرید 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>82697</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری هات نایت ز 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>82696</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری هات نایت م 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>82695</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری کرید اونتوس ایکستریم 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>82694</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری کرید اونتوس ایکستریم 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>82692</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری لولا 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>82691</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری شادو 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>82690</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری شادو 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>82688</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری شادو 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>82687</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری شادو 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>82686</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری ریور 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>82685</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری ریور 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>82683</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری ریور 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>82682</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری ریور 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>82681</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری ویند 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>82680</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری ویند 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>82678</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری ویند 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>82677</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری ویند 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>82676</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری سان 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>82675</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری سان 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>82674</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری سان 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>82673</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری سان 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>82672</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری بلاسم 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>82671</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری کارن ایکستریم 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>82670</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری مونتین 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>82669</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری مونتین 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>82668</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری مونتین 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>82667</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری مونتین 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>82665</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری مون 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>82664</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری مون 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>82663</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری مون 30  میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>82662</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری مون 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>82660</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری آمز 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>82659</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری پی اس 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>82658</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری دزرت 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>82657</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری دزرت 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>82656</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری دزرت 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>82655</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری دزرت 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>82654</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری هیرو 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>82653</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری هیرو 10 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>82650</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری کلود - 100  میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>82649</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری کلود - 50  میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>82648</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری کلود - 30  میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>82647</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری کلود - 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>82645</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری تام فورد گری وتیور 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>82644</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری دورمون - 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>82643</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری دورمون - 20 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>82642</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری دورمون - 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>82641</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری دورمون - 10 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>82640</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری سانتال - 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>82639</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری سانتال - 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>82638</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری تام فورد فاکینگ فبیولس - 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>82637</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری تام فورد فاکینگ فبیولس - 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>82636</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری تام فورد فاکینگ فبیولس - 20 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>82635</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری جورجیو - 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>82634</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری جورجیو - 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>82633</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری جادور 10 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>82568</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری باکارات رژ 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>82567</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری لیدی گاگا ایکستریم - 10 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>82566</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری لیدی گاگا - 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>82564</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری ملکول گرید دو - 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>82563</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری ملکول - 10 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>82561</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری پرادا لهوم اینتنس - 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>82560</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری پرادا لهوم اینتنس - 20 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>82027</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری جادور -  10 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>81945</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری ملکول 10 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>81112</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>پیور پرفیوم تجاری مک 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>81078</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری هیرو -  10 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>81071</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری باکارات رژ -  15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>81069</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری مون-  50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>81068</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری مون -  30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>80461</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری سان - 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>80460</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری سان - 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>80444</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری مونتین - 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>80443</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری مونتین - 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>80441</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری مونتین - 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>80439</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری ویند - 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C111" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>80437</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری ویند - 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C112" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>80436</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری ویند - 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C113" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>80434</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری ریور - 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C114" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>80433</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری ریور - 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C115" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>80432</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری ریور - 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>80430</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری شادو - 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C117" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>80428</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری شادو - 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C118" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>79761</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری جورجیو 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>79760</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری جورجیو 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C120" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>79641</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>پیور پرفیوم تجاری لیمیت 20 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C121" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>79640</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>پیور پرفیوم انحصاری دیت تایم زنانه 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C122" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>79639</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>پیور پرفیوم انحصاری دیت تایم زنانه 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C123" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>79638</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>پیور پرفیوم انحصاری دیت تایم مردانه 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C124" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>79637</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>پیور پرفیوم انحصاری دیت تایم مردانه 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C125" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>78591</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>پیور پرفیوم انحصاری لیمیتد ادیشن شماره 12 - 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C126" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>78080</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری آتس سا  - 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C127" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>77060</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری لیدی گاگا 15 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C128" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>76875</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Exclusive hair perfume هات نایت مردانه هانی مون</t>
+        </is>
+      </c>
+      <c r="C129" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>76874</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Exclusive hair perfume کارن تاپ هانی مون</t>
+        </is>
+      </c>
+      <c r="C130" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>75944</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری پرادا لهوم اینتنس 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C131" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>75942</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری پرادا لهوم اینتنس 20 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C132" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>75210</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری فاکینگ فبیولس 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C133" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>75206</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری سانتال 50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C134" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>75205</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری سانتال 30 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C135" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>74718</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم تجاری ملکول گرید دو 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C136" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>74717</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری آتس سا -  50 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C137" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>74716</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری آتس سا - 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C138" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>74700</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Exclusive hair perfume هات نایت زنانه هانی مون</t>
+        </is>
+      </c>
+      <c r="C139" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>74699</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Exclusive hair perfume هیلا هانی مون</t>
+        </is>
+      </c>
+      <c r="C140" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>74647</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری آیسو -  100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C141" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>74646</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری تارا  - 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C142" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>74645</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>نیش پرفیوم انحصاری ناشا - 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C143" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>71090</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>پیور پرفیوم تجاری ادوتویلت آمور آمور 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C144" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>68168</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>پیور پرفیوم تجاری تام فورد تاپ 100 میل هانی مون</t>
+        </is>
+      </c>
+      <c r="C145" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>